<commit_message>
Logos for NTP time, ESP time, and clear added Time source is dsplayed now (testing outstandng)
</commit_message>
<xml_diff>
--- a/MyESP/Bitmaps.xlsx
+++ b/MyESP/Bitmaps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\Arduino\MyESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juerg\Documents\_Workspaces\MyESP32\MyESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0A95DB-4C18-4299-9580-3A28FA89C065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A3A58E-022B-43BA-B1E1-E08457B17DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{275EEC98-FAE2-4C76-B66E-1C5343550326}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="7">
   <si>
     <t>b</t>
   </si>
@@ -47,7 +47,16 @@
     <t>WLAN Symbol</t>
   </si>
   <si>
-    <t>Text RTC</t>
+    <t>Symbol Timesource = RTC</t>
+  </si>
+  <si>
+    <t>Symbol Timesource = NTP</t>
+  </si>
+  <si>
+    <t>Clear Symbol</t>
+  </si>
+  <si>
+    <t>Symbol Timesource = ESP</t>
   </si>
 </sst>
 </file>
@@ -137,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,6 +162,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -489,20 +501,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A81B5E47-E8F7-4C46-932E-41EE04A3C80A}">
-  <dimension ref="A1:AS18"/>
+  <dimension ref="A1:BP27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AQ16" sqref="AQ16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="21" width="2.6328125" style="1" customWidth="1"/>
     <col min="22" max="22" width="2.6328125" customWidth="1"/>
+    <col min="23" max="23" width="5.6328125" customWidth="1"/>
     <col min="24" max="45" width="2.6328125" customWidth="1"/>
+    <col min="46" max="46" width="5.6328125" customWidth="1"/>
+    <col min="47" max="68" width="2.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A1" s="2">
         <v>0</v>
       </c>
@@ -635,8 +650,74 @@
       <c r="AS1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW1" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX1" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY1" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA1" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BC1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF1" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BI1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BJ1" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN1" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO1" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -769,8 +850,74 @@
       <c r="AS2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN2" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -903,8 +1050,74 @@
       <c r="AS3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF3" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN3" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP3" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
@@ -1037,8 +1250,74 @@
       <c r="AS4" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF4" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN4" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP4" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>0</v>
       </c>
@@ -1171,8 +1450,74 @@
       <c r="AS5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP5" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -1305,8 +1650,74 @@
       <c r="AS6" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP6" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -1439,8 +1850,74 @@
       <c r="AS7" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP7" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>0</v>
       </c>
@@ -1573,8 +2050,74 @@
       <c r="AS8" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>1</v>
+      </c>
+      <c r="AZ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BB8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BL8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN8" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP8" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>0</v>
       </c>
@@ -1707,8 +2250,74 @@
       <c r="AS9" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BK9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO9" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP9" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>0</v>
       </c>
@@ -1841,8 +2450,74 @@
       <c r="AS10" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU10" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="4">
+        <v>1</v>
+      </c>
+      <c r="BB10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="4">
+        <v>1</v>
+      </c>
+      <c r="BI10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="4">
+        <v>1</v>
+      </c>
+      <c r="BK10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="4">
+        <v>1</v>
+      </c>
+      <c r="BM10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP10" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -1975,282 +2650,1719 @@
       <c r="AS11" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AU11" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BB11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BF11" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BH11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BI11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BK11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BO11" s="4">
+        <v>1</v>
+      </c>
+      <c r="BP11" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AF12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AH12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="2"/>
-      <c r="AN12" s="2"/>
-      <c r="AO12" s="2"/>
-      <c r="AP12" s="2"/>
-      <c r="AQ12" s="2"/>
-      <c r="AR12" s="2"/>
-      <c r="AS12" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row r="13" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="X13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AB13" s="5"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AK13" s="5"/>
+      <c r="AL13" s="5"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AU13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV13" s="6"/>
+      <c r="AW13" s="6"/>
+      <c r="AX13" s="6"/>
+      <c r="AY13" s="6"/>
+      <c r="AZ13" s="6"/>
+      <c r="BA13" s="6"/>
+      <c r="BB13" s="6"/>
+      <c r="BC13" s="6"/>
+      <c r="BD13" s="6"/>
+      <c r="BE13" s="6"/>
+      <c r="BF13" s="6"/>
+      <c r="BG13" s="6"/>
+      <c r="BH13" s="6"/>
+      <c r="BI13" s="6"/>
+      <c r="BJ13" s="6"/>
+      <c r="BK13" s="6"/>
+      <c r="BL13" s="6"/>
+      <c r="BM13" s="6"/>
+      <c r="BN13" s="6"/>
+      <c r="BO13" s="6"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AF13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AN13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AR13" s="2"/>
+    <row r="14" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="1"/>
+      <c r="AO14" s="1"/>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AH14" s="2"/>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2"/>
-      <c r="AN14" s="2"/>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
+    <row r="15" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-      <c r="AG15" s="2"/>
-      <c r="AH15" s="2"/>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2"/>
-      <c r="AK15" s="2"/>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="2"/>
-      <c r="AN15" s="2"/>
-      <c r="AO15" s="2"/>
-      <c r="AP15" s="2"/>
-      <c r="AQ15" s="2"/>
-      <c r="AR15" s="2"/>
+    <row r="16" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0</v>
+      </c>
+      <c r="T16" s="4">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-      <c r="AG16" s="2"/>
-      <c r="AH16" s="2"/>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2"/>
-      <c r="AK16" s="2"/>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="2"/>
-      <c r="AN16" s="2"/>
-      <c r="AO16" s="2"/>
-      <c r="AP16" s="2"/>
-      <c r="AQ16" s="2"/>
-      <c r="AR16" s="2"/>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>0</v>
+      </c>
+      <c r="T17" s="4">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4">
+        <v>0</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS17" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="X18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
-      <c r="AJ18" s="5"/>
-      <c r="AK18" s="5"/>
-      <c r="AL18" s="5"/>
-      <c r="AM18" s="5"/>
-      <c r="AN18" s="5"/>
-      <c r="AO18" s="5"/>
-      <c r="AP18" s="5"/>
-      <c r="AQ18" s="5"/>
-      <c r="AR18" s="5"/>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
+        <v>0</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
+        <v>0</v>
+      </c>
+      <c r="S19" s="4">
+        <v>0</v>
+      </c>
+      <c r="T19" s="4">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4">
+        <v>0</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>0</v>
+      </c>
+      <c r="T20" s="4">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
+        <v>0</v>
+      </c>
+      <c r="S21" s="4">
+        <v>0</v>
+      </c>
+      <c r="T21" s="4">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4">
+        <v>0</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4">
+        <v>0</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0</v>
+      </c>
+      <c r="T22" s="4">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4">
+        <v>0</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X22" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4">
+        <v>0</v>
+      </c>
+      <c r="S23" s="4">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4">
+        <v>0</v>
+      </c>
+      <c r="U23" s="4">
+        <v>0</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4">
+        <v>0</v>
+      </c>
+      <c r="S24" s="4">
+        <v>0</v>
+      </c>
+      <c r="T24" s="4">
+        <v>0</v>
+      </c>
+      <c r="U24" s="4">
+        <v>0</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI24" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO24" s="4">
+        <v>1</v>
+      </c>
+      <c r="AP24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS24" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0</v>
+      </c>
+      <c r="P25" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>0</v>
+      </c>
+      <c r="R25" s="4">
+        <v>0</v>
+      </c>
+      <c r="S25" s="4">
+        <v>0</v>
+      </c>
+      <c r="T25" s="4">
+        <v>0</v>
+      </c>
+      <c r="U25" s="4">
+        <v>0</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI25" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AL25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO25" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AQ25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="X27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+      <c r="AO27" s="5"/>
+      <c r="AP27" s="5"/>
+      <c r="AQ27" s="5"/>
+      <c r="AR27" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A18:U18"/>
-    <mergeCell ref="X18:AR18"/>
+  <mergeCells count="5">
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="X13:AR13"/>
+    <mergeCell ref="AU13:BO13"/>
+    <mergeCell ref="A27:U27"/>
+    <mergeCell ref="X27:AR27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>